<commit_message>
Insert reviews in the review sheet instead of comments file after urgent meeting
</commit_message>
<xml_diff>
--- a/Comments file.xlsx
+++ b/Comments file.xlsx
@@ -8,17 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nadaf\Desktop\ITI\QA\QA_workshop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F0873DA7-3021-4B47-B609-58593227364A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A405FC8F-18AB-4572-A349-AEB22D0783ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1857,12 +1865,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1872,6 +1874,12 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2155,8 +2163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2425,92 +2433,92 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="48.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:5" ht="79.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="11">
+      <c r="A17" s="9">
         <v>15</v>
       </c>
-      <c r="B17" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="11" t="s">
+      <c r="B17" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E17" s="10" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="95.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="11">
+      <c r="A18" s="9">
         <v>16</v>
       </c>
-      <c r="B18" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="11" t="s">
+      <c r="B18" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" s="10" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="95.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="11">
+      <c r="A19" s="9">
         <v>17</v>
       </c>
-      <c r="B19" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="11" t="s">
+      <c r="B19" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="10" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="95.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="11">
+      <c r="A20" s="9">
         <v>18</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="11" t="s">
+      <c r="B20" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="10" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="78" x14ac:dyDescent="0.3">
-      <c r="A21" s="11">
+      <c r="A21" s="9">
         <v>19</v>
       </c>
-      <c r="B21" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="11" t="s">
+      <c r="B21" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D21" s="3" t="s">
@@ -2521,16 +2529,16 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A22" s="11">
+      <c r="A22" s="9">
         <v>20</v>
       </c>
-      <c r="B22" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="13" t="s">
+      <c r="B22" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="11" t="s">
         <v>49</v>
       </c>
       <c r="E22" s="3" t="s">
@@ -2538,16 +2546,16 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A23" s="11">
+      <c r="A23" s="9">
         <v>21</v>
       </c>
-      <c r="B23" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="13" t="s">
+      <c r="B23" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="11" t="s">
         <v>51</v>
       </c>
       <c r="E23" s="3" t="s">
@@ -2555,16 +2563,16 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A24" s="11">
+      <c r="A24" s="9">
         <v>22</v>
       </c>
-      <c r="B24" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="13" t="s">
+      <c r="B24" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="11" t="s">
         <v>50</v>
       </c>
       <c r="E24" s="3" t="s">
@@ -2572,16 +2580,16 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="11">
+      <c r="A25" s="9">
         <v>23</v>
       </c>
-      <c r="B25" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="13" t="s">
+      <c r="B25" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="11" t="s">
         <v>52</v>
       </c>
       <c r="E25" s="3" t="s">
@@ -2589,16 +2597,16 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A26" s="11">
+      <c r="A26" s="9">
         <v>24</v>
       </c>
-      <c r="B26" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="13" t="s">
+      <c r="B26" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="11" t="s">
         <v>53</v>
       </c>
       <c r="E26" s="3" t="s">
@@ -2606,16 +2614,16 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A27" s="11">
+      <c r="A27" s="9">
         <v>25</v>
       </c>
-      <c r="B27" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="13" t="s">
+      <c r="B27" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="11" t="s">
         <v>58</v>
       </c>
       <c r="E27" s="3" t="s">
@@ -2623,16 +2631,16 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A28" s="11">
+      <c r="A28" s="9">
         <v>26</v>
       </c>
-      <c r="B28" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="13" t="s">
+      <c r="B28" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="11" t="s">
         <v>59</v>
       </c>
       <c r="E28" s="3" t="s">
@@ -2640,16 +2648,16 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A29" s="11">
+      <c r="A29" s="9">
         <v>27</v>
       </c>
-      <c r="B29" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="14" t="s">
+      <c r="B29" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="12" t="s">
         <v>60</v>
       </c>
       <c r="E29" s="3" t="s">
@@ -2657,16 +2665,16 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A30" s="11">
+      <c r="A30" s="9">
         <v>28</v>
       </c>
-      <c r="B30" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="14" t="s">
+      <c r="B30" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="12" t="s">
         <v>61</v>
       </c>
       <c r="E30" s="3" t="s">
@@ -2674,16 +2682,16 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A31" s="11">
+      <c r="A31" s="9">
         <v>30</v>
       </c>
-      <c r="B31" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="13" t="s">
+      <c r="B31" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="11" t="s">
         <v>62</v>
       </c>
       <c r="E31" s="3" t="s">
@@ -2691,16 +2699,16 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A32" s="11">
+      <c r="A32" s="9">
         <v>31</v>
       </c>
-      <c r="B32" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="14" t="s">
+      <c r="B32" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="12" t="s">
         <v>65</v>
       </c>
       <c r="E32" s="3" t="s">
@@ -2708,16 +2716,16 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="97.2" x14ac:dyDescent="0.3">
-      <c r="A33" s="11">
+      <c r="A33" s="9">
         <v>32</v>
       </c>
-      <c r="B33" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="14" t="s">
+      <c r="B33" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="12" t="s">
         <v>68</v>
       </c>
       <c r="E33" s="7" t="s">
@@ -2725,13 +2733,13 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="64.2" x14ac:dyDescent="0.3">
-      <c r="A34" s="11">
+      <c r="A34" s="9">
         <v>33</v>
       </c>
-      <c r="B34" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C34" s="11" t="s">
+      <c r="B34" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D34" s="2" t="s">

</xml_diff>

<commit_message>
updating layouts after removing feedback section
</commit_message>
<xml_diff>
--- a/Comments file.xlsx
+++ b/Comments file.xlsx
@@ -2,19 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITI\QA project Team D\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\QA Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="13170"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="45">
   <si>
     <t>Comment ID</t>
   </si>
@@ -46,13 +46,134 @@
     <t>Comment By</t>
   </si>
   <si>
-    <t xml:space="preserve">Comment In </t>
+    <t>Comment date</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>Assigned to</t>
+  </si>
+  <si>
+    <t>close date</t>
+  </si>
+  <si>
+    <t>comment_01</t>
+  </si>
+  <si>
+    <t>comment_02</t>
+  </si>
+  <si>
+    <t>comment_03</t>
+  </si>
+  <si>
+    <t>comment_04</t>
+  </si>
+  <si>
+    <t>comment_05</t>
+  </si>
+  <si>
+    <t>comment_06</t>
+  </si>
+  <si>
+    <t>comment_07</t>
+  </si>
+  <si>
+    <t>comment_08</t>
+  </si>
+  <si>
+    <t>comment_09</t>
+  </si>
+  <si>
+    <t>comment_10</t>
+  </si>
+  <si>
+    <t>comment_11</t>
+  </si>
+  <si>
+    <t>comment_12</t>
+  </si>
+  <si>
+    <t>comment_13</t>
+  </si>
+  <si>
+    <t>comment_14</t>
+  </si>
+  <si>
+    <t>Amr Mokhtar</t>
+  </si>
+  <si>
+    <t>No document revision table in the PMP</t>
+  </si>
+  <si>
+    <t>PMP</t>
+  </si>
+  <si>
+    <t>the timeline of the project only mentions 5 weeks no specific date</t>
+  </si>
+  <si>
+    <t>the CM plan isn't defined</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> please add more details into escalation seciton</t>
+  </si>
+  <si>
+    <t>PMP only reviewed once by the team and the comments from customer not added</t>
+  </si>
+  <si>
+    <t>multiple uploads while only 2 reviews are done</t>
+  </si>
+  <si>
+    <t>no review strategy is unified the requirements are reviewed not by checklist.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> how you will handle more than one review of PMP
+Tracibility</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> only SRS has IDS it should be all levels</t>
+  </si>
+  <si>
+    <t>SRS</t>
+  </si>
+  <si>
+    <t>REQ-11Signup is vague</t>
+  </si>
+  <si>
+    <t>only one version is added in the version control on 14/4 but the document was updated after that date.</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>no interfaces between modules</t>
+  </si>
+  <si>
+    <t>no modules of the system</t>
+  </si>
+  <si>
+    <t>LLD is missing</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>SMP</t>
+  </si>
+  <si>
+    <t>reviews</t>
+  </si>
+  <si>
+    <t>Tracibility matrix</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -99,29 +220,6 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
-      <color theme="5" tint="-0.499984740745262"/>
-      <name val="Calibri Light"/>
-      <family val="1"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri Light"/>
-      <family val="1"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
       <sz val="16"/>
       <color theme="4" tint="-0.499984740745262"/>
       <name val="Calibri Light"/>
@@ -134,6 +232,27 @@
       <color rgb="FF002060"/>
       <name val="Calibri Light"/>
       <family val="1"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
       <scheme val="major"/>
     </font>
   </fonts>
@@ -169,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -180,16 +299,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -197,17 +307,41 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -489,269 +623,462 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.88671875" customWidth="1"/>
-    <col min="2" max="2" width="37" customWidth="1"/>
-    <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="44.77734375" customWidth="1"/>
-    <col min="5" max="5" width="48.6640625" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="68.140625" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="26.85546875" customWidth="1"/>
+    <col min="8" max="8" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="9" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" ht="48.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="12"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-    </row>
-    <row r="17" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
+      <c r="F1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="15">
+        <v>44685</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="16">
+        <v>44685</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="16">
+        <v>44685</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="16">
+        <v>44685</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="16">
+        <v>44685</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="17">
+        <v>44685</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="17">
+        <v>44685</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="16">
+        <v>44685</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="16">
+        <v>44685</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="16">
+        <v>44685</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="16">
+        <v>44685</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="16">
+        <v>44685</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="16">
+        <v>44685</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="16">
+        <v>44685</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="48.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="10"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="9"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="9"/>
-    </row>
-    <row r="19" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
       <c r="D19" s="2"/>
-      <c r="E19" s="9"/>
-    </row>
-    <row r="20" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="9"/>
-    </row>
-    <row r="21" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="10"/>
+    <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="7"/>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="10"/>
+    <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="7"/>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="10"/>
+    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="7"/>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="10"/>
+    <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="7"/>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="10"/>
+    <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="7"/>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="10"/>
+    <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="7"/>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="10"/>
+    <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="7"/>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="11"/>
+    <row r="29" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="8"/>
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="11"/>
+    <row r="30" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="8"/>
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="10"/>
+    <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="7"/>
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="11"/>
+    <row r="32" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="8"/>
       <c r="E32" s="3"/>
     </row>
-    <row r="33" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="6"/>
-    </row>
-    <row r="34" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
+    <row r="33" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
       <c r="D34" s="2"/>
       <c r="E34" s="3"/>
     </row>

</xml_diff>